<commit_message>
Corrected mistake of country attribution and added Dorgeist
</commit_message>
<xml_diff>
--- a/data/processed/land_sink_by_country.xlsx
+++ b/data/processed/land_sink_by_country.xlsx
@@ -448,1848 +448,1848 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>MAR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.5371012036145594</t>
+          <t>-0.0031559210162951214</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGO</t>
+          <t>DZA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.05223984680089482</t>
+          <t>-0.0024231829030629958</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ALB</t>
+          <t>STP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.001011609366382621</t>
+          <t>-0.000423021423724358</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AND</t>
+          <t>ATG</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.7856088614346858e-05</t>
+          <t>-0.0002977279758491523</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ARE</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.0001252895933168955</t>
+          <t>-0.00018177878398285951</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ARG</t>
+          <t>OMN</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.054387216933544376</t>
+          <t>-0.00012769889261987264</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ARM</t>
+          <t>TLS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.00014006664846226392</t>
+          <t>-9.9489041928082e-05</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ATG</t>
+          <t>KNA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8.657307501785884e-08</t>
+          <t>-2.7338137852053907e-05</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>KWT</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.03927547134740918</t>
+          <t>-3.7030984342155574e-06</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AUT</t>
+          <t>MCO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.002743985149051558</t>
+          <t>-7.724357334734308e-09</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AZE</t>
+          <t>VAT</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.000662189161303243</t>
+          <t>4.409335239164555e-09</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BDI</t>
+          <t>SMR</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.0013973180609668547</t>
+          <t>3.313519513883484e-07</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>LIE</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.0002309345127770423</t>
+          <t>3.8619501910635045e-06</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BEN</t>
+          <t>LUX</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.001604669044020905</t>
+          <t>4.095414092019309e-06</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BFA</t>
+          <t>BHR</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0.0037123795828507165</t>
+          <t>9.205654720758924e-06</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BGD</t>
+          <t>MLT</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.007723249741700458</t>
+          <t>1.6929096919123816e-05</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AND</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.004142109499616741</t>
+          <t>1.7856088614346858e-05</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BHR</t>
+          <t>DJI</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>9.205654720758924e-06</t>
+          <t>2.6765199692620304e-05</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BHS</t>
+          <t>GRD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.0034214757884954514</t>
+          <t>6.900477526471112e-05</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BIH</t>
+          <t>SGP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0.0017774925681813703</t>
+          <t>6.933036984835678e-05</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>QAT</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.006585970355338423</t>
+          <t>8.40361348266287e-05</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BLZ</t>
+          <t>PSE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0.0026565029509685993</t>
+          <t>8.988656038449994e-05</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BOL</t>
+          <t>ARE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0.029704648608806818</t>
+          <t>0.00013318622563672858</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BRA</t>
+          <t>ARM</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.2929627848407269</t>
+          <t>0.00014006664846226392</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BRB</t>
+          <t>GMB</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>-5.5263524626077074e-05</t>
+          <t>0.00019268151587515487</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BRN</t>
+          <t>JOR</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0.0008483740328460015</t>
+          <t>0.00021087684616415757</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>DMA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.0018656598200831062</t>
+          <t>0.00022354964980172073</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BWA</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0.005634140573959298</t>
+          <t>0.0002309345127770423</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CAF</t>
+          <t>ISR</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.029865573254712223</t>
+          <t>0.00023373829684297668</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>BRB</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0.2260957150333586</t>
+          <t>0.0002562328104108902</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CHE</t>
+          <t>LBN</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0.001001032598654716</t>
+          <t>0.00026680314204506546</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CHL</t>
+          <t>NRU</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>0.013436784535552481</t>
+          <t>0.00033012359667162924</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>MDA</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0.25644570478635825</t>
+          <t>0.000343783699081745</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CIV</t>
+          <t>SYC</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0.012223512485266607</t>
+          <t>0.0003549537937603416</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CMR</t>
+          <t>NIU</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0.024880930990905662</t>
+          <t>0.0003794745085967165</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>COD</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>0.18758371935431564</t>
+          <t>0.0004963969976217436</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>COG</t>
+          <t>MDV</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>0.023781627502660052</t>
+          <t>0.0004991185466960407</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>VCT</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0.001674439965114975</t>
+          <t>0.0005245645279905648</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>LSO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0.060329817040999476</t>
+          <t>0.0005442979034521379</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>COM</t>
+          <t>MNE</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8.455362180941092e-05</t>
+          <t>0.0005853418648603405</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CPV</t>
+          <t>CYP</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>0.0002423480678745445</t>
+          <t>0.0006211059332811503</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CRI</t>
+          <t>MHL</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.005560458468209595</t>
+          <t>0.0006401547526481806</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CUB</t>
+          <t>CPV</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0.008022651129568828</t>
+          <t>0.0006907808517682092</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CYP</t>
+          <t>SWZ</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0.0003035609776950005</t>
+          <t>0.0007716321705752557</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CZE</t>
+          <t>SVN</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>0.001016598664050661</t>
+          <t>0.0007815140974888758</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DEU</t>
+          <t>LBY</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>0.002090229210504407</t>
+          <t>0.0008468203290671601</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DISPUTED</t>
+          <t>MUS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.009881486933196208</t>
+          <t>0.0008543218110631549</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DJI</t>
+          <t>CHE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2.6765199692620304e-05</t>
+          <t>0.001001032598654716</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DMA</t>
+          <t>ALB</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7.5116905672639e-05</t>
+          <t>0.0010011268541240568</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DNK</t>
+          <t>SAU</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>0.0027339833673578604</t>
+          <t>0.001008581814774199</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DOM</t>
+          <t>CZE</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>0.0031832294771150897</t>
+          <t>0.001016598664050661</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DZA</t>
+          <t>MKD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>-0.002410592766390486</t>
+          <t>0.0010255207627002294</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ECU</t>
+          <t>AZE</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>0.016482322806392113</t>
+          <t>0.0010258373960378923</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>EGY</t>
+          <t>PLW</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>0.000819415244512608</t>
+          <t>0.001028102800173753</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ERI</t>
+          <t>GNB</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>0.0021975890456139395</t>
+          <t>0.0010508781854131658</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ESP</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>0.008446786939038813</t>
+          <t>0.001085752017724851</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>EST</t>
+          <t>FSM</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>0.0022805759423695114</t>
+          <t>0.0011259983249157575</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ETH</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>0.051499334066337776</t>
+          <t>0.001166018476496812</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>FIN</t>
+          <t>MRT</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>0.011010783902081293</t>
+          <t>0.0011944392539647631</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>FJI</t>
+          <t>SVK</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.004642213587538295</t>
+          <t>0.0012045565414064137</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>EGY</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>0.01609725873143701</t>
+          <t>0.0012049210439857272</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>FSM</t>
+          <t>HUN</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>0.0009501275363493396</t>
+          <t>0.0012462300249546333</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>GAB</t>
+          <t>IRQ</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>0.019656520998804446</t>
+          <t>0.0012662892732907922</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>GBR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>0.006592960619137075</t>
+          <t>0.0013242716524631125</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>NLD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.001756338647448897</t>
+          <t>0.0013339868057889274</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>GHA</t>
+          <t>BRN</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.008127037373103989</t>
+          <t>0.001370304087310789</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>GIN</t>
+          <t>SYR</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.008652372956331943</t>
+          <t>0.0013786021815525296</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>GMB</t>
+          <t>BDI</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.00019268151587515487</t>
+          <t>0.0013973180609668547</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>GNB</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.0009562128429294867</t>
+          <t>0.001415565621363806</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>GNQ</t>
+          <t>TGO</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.0021050450545474614</t>
+          <t>0.0014200688013930477</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>GRC</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>0.007771108662829644</t>
+          <t>0.001499980627931268</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>GRD</t>
+          <t>TUV</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1.8417516472739413e-05</t>
+          <t>0.0015612143125389734</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>GTM</t>
+          <t>SLV</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>0.008067347544441335</t>
+          <t>0.0015784105189922068</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>GUY</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>0.015951522976332042</t>
+          <t>0.0016493693106853031</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>HND</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>0.009007302775733896</t>
+          <t>0.0016768879007607008</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>HRV</t>
+          <t>TTO</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>0.002024535824669106</t>
+          <t>0.0016846147082373564</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>HTI</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>0.0013424187963088131</t>
+          <t>0.0017213169082839614</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>HUN</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.0012462300249546333</t>
+          <t>0.0017264378650334441</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>IDN</t>
+          <t>YEM</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>0.24428008723423272</t>
+          <t>0.0017310549706899703</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>BEN</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>0.13801153605178065</t>
+          <t>0.0017410195651943873</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IRL</t>
+          <t>BIH</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.002033734174706874</t>
+          <t>0.0017774925681813703</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>IRN</t>
+          <t>ISL</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.0028019542507220344</t>
+          <t>0.0018085261597327448</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>IRQ</t>
+          <t>BTN</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>0.0012662892732907922</t>
+          <t>0.0018656598200831062</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ISL</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.0014844815476059159</t>
+          <t>0.002106218046861762</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ISR</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>0.00018729578086979672</t>
+          <t>0.0021305903406599424</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ITA</t>
+          <t>SEN</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.0032903037812051362</t>
+          <t>0.0021455173629216302</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>JAM</t>
+          <t>ERI</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>0.000890955487087474</t>
+          <t>0.0022152699727711806</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>JOR</t>
+          <t>HRV</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.00021087684616415757</t>
+          <t>0.00221802235944</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>JPN</t>
+          <t>GNQ</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>0.03318042824096012</t>
+          <t>0.00224927490149473</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>KAZ</t>
+          <t>HTI</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.02201722639265566</t>
+          <t>0.0023312014314916855</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>KEN</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>0.038029578545954304</t>
+          <t>0.00242735122694895</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>KGZ</t>
+          <t>LTU</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>0.003317906634814413</t>
+          <t>0.002461845316850536</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>KHM</t>
+          <t>JAM</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>0.013159119247020856</t>
+          <t>0.0025099571166191494</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>KIR</t>
+          <t>EST</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.0026821319829010096</t>
+          <t>0.002522954316000542</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>KNA</t>
+          <t>IRL</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>-2.7338137852053907e-05</t>
+          <t>0.0026433944753224145</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>KOR</t>
+          <t>AUT</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>0.009173871260516105</t>
+          <t>0.002743985149051558</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>KWT</t>
+          <t>IRN</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>-6.183475443611315e-06</t>
+          <t>0.003017780127614397</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>LVA</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>0.01641877943268011</t>
+          <t>0.003198006219070156</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LBN</t>
+          <t>KGZ</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.00019178486508743912</t>
+          <t>0.003317906634814413</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LBR</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>0.007498827041392301</t>
+          <t>0.003337439968785063</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>LBY</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>0.00031168279280850534</t>
+          <t>0.0035004222745695763</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>BLZ</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>0.00037627475881639574</t>
+          <t>0.0036462337981488908</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>LIE</t>
+          <t>DNK</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>3.8619501910635045e-06</t>
+          <t>0.0036662145383867255</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>LKA</t>
+          <t>BFA</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>0.007679339417324342</t>
+          <t>0.0037123795828507165</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>LSO</t>
+          <t>AFG</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>0.0005442979034521379</t>
+          <t>0.0037834464244554424</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>LTU</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>0.002461845316850536</t>
+          <t>0.0040708195236845825</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>MWI</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>4.095414092019309e-06</t>
+          <t>0.004129937345873757</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>LVA</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>0.002961274648783733</t>
+          <t>0.00459609060293472</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>MAR</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>-0.0030475500614694268</t>
+          <t>0.004709895969265818</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>MCO</t>
+          <t>ROU</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>-7.724357334734308e-09</t>
+          <t>0.004878883414850368</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>MDA</t>
+          <t>KIR</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>0.000343783699081745</t>
+          <t>0.005201401530993579</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>MDG</t>
+          <t>SLE</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>0.020224543926652475</t>
+          <t>0.005411510156226266</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>MDV</t>
+          <t>POL</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>0.0004991185466960407</t>
+          <t>0.005516558517029448</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MLI</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>0.06876564133544631</t>
+          <t>0.0055265755303689785</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>MHL</t>
+          <t>BWA</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>0.0006401547526481806</t>
+          <t>0.005634140573959298</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>MKD</t>
+          <t>PAK</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>0.0010255207627002294</t>
+          <t>0.006147746616711429</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>MLI</t>
+          <t>DOM</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>0.0055265755303689785</t>
+          <t>0.006368342812152397</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>MLT</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2.9369701638504312e-05</t>
+          <t>0.006585970355338423</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>MMR</t>
+          <t>TCD</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>0.047923531538212716</t>
+          <t>0.006669625075029828</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>MNE</t>
+          <t>FJI</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>0.0005853418648603405</t>
+          <t>0.006965395989656404</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>MNG</t>
+          <t>NPL</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>0.01426401856497548</t>
+          <t>0.0076507437056719165</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>MOZ</t>
+          <t>GIN</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>0.025618677175684924</t>
+          <t>0.007871979054485334</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>MRT</t>
+          <t>BHS</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>0.0011824364264092944</t>
+          <t>0.008038846776898135</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>MUS</t>
+          <t>GHA</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>0.00023575416091365896</t>
+          <t>0.008634430122893146</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>MWI</t>
+          <t>ZWE</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>0.004129937345873757</t>
+          <t>0.008641773312755289</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>MYS</t>
+          <t>GRC</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>0.03350832662978987</t>
+          <t>0.008685293006232754</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>0.0029556498655810373</t>
+          <t>0.008706726333369762</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>NER</t>
+          <t>BGD</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>0.0035004222745695763</t>
+          <t>0.008717440766207361</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>NGA</t>
+          <t>CRI</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>0.02326260997348315</t>
+          <t>0.009156656532158166</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>NIC</t>
+          <t>GTM</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>0.010192174936182965</t>
+          <t>0.009237727254066146</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>NIU</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>-0.00017693408659758995</t>
+          <t>0.009546848609793816</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>NLD</t>
+          <t>GBR</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>0.0007405204935592238</t>
+          <t>0.009853441765618962</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>NOR</t>
+          <t>SOM</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>0.009967108900963806</t>
+          <t>0.01004025430899609</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>NPL</t>
+          <t>VUT</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>0.0076507437056719165</t>
+          <t>0.01007692562916193</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>NRU</t>
+          <t>LBR</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>0.00019941552859976288</t>
+          <t>0.010134708210078508</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>NZL</t>
+          <t>ZAF</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>0.016621426089990655</t>
+          <t>0.010291230642545297</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>OMN</t>
+          <t>PRY</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>-0.00012193457693573988</t>
+          <t>0.010298068948164324</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>HND</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>0.00024440440339048935</t>
+          <t>0.010931429294657492</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>PAK</t>
+          <t>URY</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>0.006093368758833344</t>
+          <t>0.011037107802874957</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>ESP</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>0.01031793718129441</t>
+          <t>0.011187484239717764</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOR</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>0.06218400225958789</t>
+          <t>0.011387774839169279</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>FIN</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>0.04462092261632685</t>
+          <t>0.011874802397117579</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>PLW</t>
+          <t>CUB</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>0.0007043443932829999</t>
+          <t>0.012757243456667147</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>PNG</t>
+          <t>DISPUTED</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>0.06516704945836307</t>
+          <t>0.01290375121370114</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>POL</t>
+          <t>NIC</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>0.005191619925924647</t>
+          <t>0.012915394756461123</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>PRK</t>
+          <t>KOR</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>0.007431556680931888</t>
+          <t>0.013784513598452224</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>KHM</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>0.0033420071464785378</t>
+          <t>0.013810177471643743</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>PRY</t>
+          <t>CIV</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>0.010298068948164324</t>
+          <t>0.014163678840356235</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>PSE</t>
+          <t>MNG</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>8.988656038449994e-05</t>
+          <t>0.01426401856497548</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>QAT</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>6.270011258128986e-05</t>
+          <t>0.01477305902568124</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ROU</t>
+          <t>LKA</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>0.0047215227022316675</t>
+          <t>0.014985206379070222</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>ECU</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>0.413783319928225</t>
+          <t>0.015804137261332063</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>SUR</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>0.001415565621363806</t>
+          <t>0.015819192010425677</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>SAU</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>0.0009796998283368853</t>
+          <t>0.01599871869169472</t>
         </is>
       </c>
     </row>
@@ -2301,535 +2301,535 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>0.016148990806438536</t>
+          <t>0.016190883040850704</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>SEN</t>
+          <t>CHL</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>0.0019705830502322287</t>
+          <t>0.016402838561838065</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>SGP</t>
+          <t>LAO</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>6.933036984835678e-05</t>
+          <t>0.01641877943268011</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>SLB</t>
+          <t>SWE</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>0.012064323849884782</t>
+          <t>0.01847961918387613</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>SLE</t>
+          <t>GUY</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>0.004723507986841527</t>
+          <t>0.01858434819230957</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>SLV</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>0.0012051024797029184</t>
+          <t>0.01887511732410361</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>SMR</t>
+          <t>GAB</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>3.313519513883484e-07</t>
+          <t>0.020834888092829316</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>SOM</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>0.00947237674415589</t>
+          <t>0.02085258748181859</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>KAZ</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>0.00242735122694895</t>
+          <t>0.02204948449275636</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>SSD</t>
+          <t>TUR</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>0.01887511732410361</t>
+          <t>0.023722825740888662</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>STP</t>
+          <t>COG</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>-4.884182468790846e-05</t>
+          <t>0.024120441045493313</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>SUR</t>
+          <t>NGA</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>0.012466321377913604</t>
+          <t>0.024690771495892293</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>SVK</t>
+          <t>CMR</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>0.0012045565414064137</t>
+          <t>0.024959655340726108</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>VEN</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>0.0007815140974888758</t>
+          <t>0.025693916544896018</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>SWE</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>0.01650135066799819</t>
+          <t>0.02619336605720143</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>SWZ</t>
+          <t>NZL</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>0.0007716321705752557</t>
+          <t>0.026484810635776616</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>SYC</t>
+          <t>BOL</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>0.00043050339048722355</t>
+          <t>0.029704648608806818</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>SYR</t>
+          <t>CAF</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>0.0013381561936286247</t>
+          <t>0.029865573254712223</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>TCD</t>
+          <t>MDG</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>0.006669625075029828</t>
+          <t>0.03294324619539568</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>TGO</t>
+          <t>ZMB</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>0.0014200688013930477</t>
+          <t>0.03306321308753948</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>THA</t>
+          <t>VNM</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>0.03489453644466156</t>
+          <t>0.03650465974901972</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>MOZ</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>0.0016768879007607008</t>
+          <t>0.03792557590019237</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>KEN</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>0.0013456474389445664</t>
+          <t>0.04112308672773814</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>TLS</t>
+          <t>THA</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>0.00031042210955029725</t>
+          <t>0.04369497763644991</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>MYS</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>0.0010532419055035564</t>
+          <t>0.0480968763028997</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>TTO</t>
+          <t>JPN</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>0.0007566328394300166</t>
+          <t>0.048376104134776825</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>ETH</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>-0.00029203784479882604</t>
+          <t>0.051499334066337776</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>TUR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>0.020417627653663464</t>
+          <t>0.05214840503684565</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>TUV</t>
+          <t>AGO</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>0.0013127823742241883</t>
+          <t>0.052595336182457056</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>TZA</t>
+          <t>MMR</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>0.04988021301563124</t>
+          <t>0.05337417069587747</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TZA</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>0.01477305902568124</t>
+          <t>0.056174023180418635</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>ARG</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>0.008261300063943522</t>
+          <t>0.05819254061919442</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>URY</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>0.009877268542700416</t>
+          <t>0.0622433506439139</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>0.31748623893167793</t>
+          <t>0.06431659982937232</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>0.0017213169082839614</t>
+          <t>0.071314580589668</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>VAT</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>4.409335239164555e-09</t>
+          <t>0.08089096718404853</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>VCT</t>
+          <t>PNG</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>0.00017256239495225286</t>
+          <t>0.09559143946644622</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>VEN</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>0.024454096884800162</t>
+          <t>0.16294438849625825</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>VNM</t>
+          <t>COD</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>0.027583687783634025</t>
+          <t>0.18758371935431564</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>VUT</t>
+          <t>CAN</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>0.005453315196911194</t>
+          <t>0.23738086479339793</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>CHN</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>0.0006071434708614881</t>
+          <t>0.2722951830124945</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>YEM</t>
+          <t>BRA</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>0.0013773255794716653</t>
+          <t>0.30985551579018894</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>ZAF</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>0.010831345064819501</t>
+          <t>0.3428953357607158</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>ZMB</t>
+          <t>IDN</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>0.03306321308753948</t>
+          <t>0.3452499029092127</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>ZWE</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>0.008641773312755289</t>
+          <t>0.4346374389525834</t>
         </is>
       </c>
     </row>

</xml_diff>